<commit_message>
add even more participants
</commit_message>
<xml_diff>
--- a/Participants.xlsx
+++ b/Participants.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinspollack9/Documents/DataScienceWorkshops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29898F31-9049-A049-9A24-1043B23CA844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8B5DE4-0439-8D4A-A257-7983F8425A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18960" yWindow="460" windowWidth="14740" windowHeight="16600" xr2:uid="{DA4AE812-50A2-7847-969A-17A7919387A9}"/>
+    <workbookView xWindow="14060" yWindow="460" windowWidth="14740" windowHeight="16580" xr2:uid="{DA4AE812-50A2-7847-969A-17A7919387A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="112">
   <si>
     <t>Adriana Coman</t>
   </si>
@@ -356,6 +356,21 @@
   </si>
   <si>
     <t>DASIL</t>
+  </si>
+  <si>
+    <t>Ioanna Giannakou</t>
+  </si>
+  <si>
+    <t>Zeineb Mezghanni</t>
+  </si>
+  <si>
+    <t>Kripa Bansal</t>
+  </si>
+  <si>
+    <t>Trung Le</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -707,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78848AA8-4587-8B45-952A-1A517872DE7C}">
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,11 +776,11 @@
       </c>
       <c r="E4">
         <f xml:space="preserve"> COUNTIF(B:B, "x")</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F4">
         <f xml:space="preserve"> COUNTIF(C:C, "x")</f>
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1042,7 +1057,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
         <v>83</v>
@@ -1050,7 +1065,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
         <v>83</v>
@@ -1058,15 +1073,15 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C42" t="s">
         <v>83</v>
@@ -1074,23 +1089,23 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>28</v>
-      </c>
-      <c r="B43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C45" t="s">
         <v>83</v>
@@ -1098,15 +1113,15 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
         <v>83</v>
@@ -1114,7 +1129,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B48" t="s">
         <v>83</v>
@@ -1122,39 +1137,39 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>33</v>
-      </c>
-      <c r="C49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>36</v>
-      </c>
-      <c r="B51" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>102</v>
-      </c>
-      <c r="C52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B53" t="s">
         <v>83</v>
@@ -1162,7 +1177,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="C54" t="s">
         <v>83</v>
@@ -1170,39 +1185,39 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>74</v>
-      </c>
-      <c r="C55" t="s">
+        <v>37</v>
+      </c>
+      <c r="B55" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>39</v>
-      </c>
-      <c r="B56" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>1</v>
-      </c>
-      <c r="B57" t="s">
+        <v>74</v>
+      </c>
+      <c r="C57" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>56</v>
-      </c>
-      <c r="C58" t="s">
+        <v>39</v>
+      </c>
+      <c r="B58" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="B59" t="s">
         <v>83</v>
@@ -1210,23 +1225,23 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>64</v>
-      </c>
-      <c r="B60" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>34</v>
-      </c>
-      <c r="C61" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
         <v>83</v>
@@ -1234,39 +1249,39 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>42</v>
-      </c>
-      <c r="B63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>43</v>
-      </c>
-      <c r="C64" t="s">
+        <v>40</v>
+      </c>
+      <c r="B64" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>44</v>
-      </c>
-      <c r="C65" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>45</v>
-      </c>
-      <c r="B66" t="s">
+        <v>43</v>
+      </c>
+      <c r="C66" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="C67" t="s">
         <v>83</v>
@@ -1274,7 +1289,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B68" t="s">
         <v>83</v>
@@ -1282,7 +1297,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C69" t="s">
         <v>83</v>
@@ -1290,15 +1305,15 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>94</v>
-      </c>
-      <c r="C70" t="s">
+        <v>46</v>
+      </c>
+      <c r="B70" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="C71" t="s">
         <v>83</v>
@@ -1306,7 +1321,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="C72" t="s">
         <v>83</v>
@@ -1314,47 +1329,47 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>65</v>
-      </c>
-      <c r="B73" t="s">
+        <v>47</v>
+      </c>
+      <c r="C73" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>60</v>
-      </c>
-      <c r="B74" t="s">
+        <v>48</v>
+      </c>
+      <c r="C74" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>49</v>
-      </c>
-      <c r="C75" t="s">
+        <v>65</v>
+      </c>
+      <c r="B75" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>50</v>
-      </c>
-      <c r="C76" t="s">
+        <v>60</v>
+      </c>
+      <c r="B76" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>67</v>
-      </c>
-      <c r="B77" t="s">
+        <v>49</v>
+      </c>
+      <c r="C77" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C78" t="s">
         <v>83</v>
@@ -1362,7 +1377,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B79" t="s">
         <v>83</v>
@@ -1370,7 +1385,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C80" t="s">
         <v>83</v>
@@ -1378,15 +1393,15 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>69</v>
-      </c>
-      <c r="C81" t="s">
+        <v>66</v>
+      </c>
+      <c r="B81" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C82" t="s">
         <v>83</v>
@@ -1394,39 +1409,39 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>70</v>
-      </c>
-      <c r="B83" t="s">
+        <v>69</v>
+      </c>
+      <c r="C83" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>89</v>
-      </c>
-      <c r="B84" t="s">
+        <v>95</v>
+      </c>
+      <c r="C84" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>71</v>
-      </c>
-      <c r="C85" t="s">
+        <v>70</v>
+      </c>
+      <c r="B85" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>93</v>
-      </c>
-      <c r="C86" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C87" t="s">
         <v>83</v>
@@ -1434,15 +1449,15 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>73</v>
-      </c>
-      <c r="B88" t="s">
+        <v>93</v>
+      </c>
+      <c r="C88" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C89" t="s">
         <v>83</v>
@@ -1450,47 +1465,47 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>76</v>
-      </c>
-      <c r="C90" t="s">
+        <v>73</v>
+      </c>
+      <c r="B90" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>96</v>
-      </c>
-      <c r="B91" t="s">
+        <v>75</v>
+      </c>
+      <c r="C91" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>77</v>
-      </c>
-      <c r="B92" t="s">
+        <v>76</v>
+      </c>
+      <c r="C92" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>90</v>
-      </c>
-      <c r="C93" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>85</v>
-      </c>
-      <c r="C94" t="s">
+        <v>77</v>
+      </c>
+      <c r="B94" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C95" t="s">
         <v>83</v>
@@ -1498,39 +1513,39 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>79</v>
-      </c>
-      <c r="B96" t="s">
+        <v>85</v>
+      </c>
+      <c r="C96" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>57</v>
-      </c>
-      <c r="B97" t="s">
+        <v>78</v>
+      </c>
+      <c r="C97" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="C98" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>86</v>
-      </c>
-      <c r="C99" t="s">
+        <v>79</v>
+      </c>
+      <c r="B99" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="B100" t="s">
         <v>83</v>
@@ -1538,7 +1553,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="C101" t="s">
         <v>83</v>
@@ -1546,15 +1561,47 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>86</v>
+      </c>
+      <c r="C102" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>81</v>
+      </c>
+      <c r="B103" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>52</v>
+      </c>
+      <c r="C104" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>58</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C105" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>108</v>
+      </c>
+      <c r="C106" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C103">
-    <sortCondition ref="A2:A103"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C106">
+    <sortCondition ref="A2:A106"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>